<commit_message>
update : check xlsx
</commit_message>
<xml_diff>
--- a/Android/03_基本設計書(Android).xlsx
+++ b/Android/03_基本設計書(Android).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2220241\AndroidStudioProjects\Whisper\Android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2220177\AndroidStudioProjects\Whisper\Android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635FD6A4-0FF3-499D-9589-78C6C9346906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5669DB4-30F0-4655-A999-9E1F44595457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="画面機能一覧" sheetId="17" r:id="rId1"/>
@@ -4611,7 +4611,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4704,9 +4704,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -4720,9 +4717,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4738,15 +4740,6 @@
     <xf numFmtId="56" fontId="7" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4756,15 +4749,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -5618,9 +5619,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5658,9 +5659,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5693,9 +5694,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5728,9 +5746,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5907,48 +5942,48 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.8"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="11"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="5"/>
-    <col min="7" max="7" width="27.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="3.54296875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.54296875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" style="5"/>
+    <col min="7" max="7" width="27.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>476</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="2" spans="1:5" ht="26.4" customHeight="1">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
         <v>472</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="40" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="39" t="s">
         <v>474</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="51">
         <v>45008</v>
       </c>
-      <c r="E2" s="48"/>
-    </row>
-    <row r="4" spans="1:5" ht="11.4" thickBot="1">
+      <c r="E2" s="50"/>
+    </row>
+    <row r="4" spans="1:5" ht="11.5" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>57</v>
       </c>
@@ -5965,20 +6000,20 @@
         <v>473</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" ht="12.6" thickTop="1">
+    <row r="5" spans="1:5" s="9" customFormat="1" ht="12.5" thickTop="1">
       <c r="A5" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="60" t="s">
         <v>477</v>
       </c>
     </row>
@@ -5997,35 +6032,35 @@
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" s="60" customFormat="1" ht="12">
-      <c r="A7" s="57">
+    <row r="7" spans="1:5" s="46" customFormat="1" ht="12">
+      <c r="A7" s="43">
         <v>3</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="59"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" spans="1:5" s="9" customFormat="1" ht="12">
       <c r="A8" s="10">
         <v>4</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:5" s="9" customFormat="1" ht="12">
       <c r="A9" s="10">
@@ -6106,16 +6141,16 @@
       <c r="A14" s="10">
         <v>10</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="45" t="s">
         <v>478</v>
       </c>
     </row>
@@ -6175,14 +6210,14 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="43"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:5" s="9" customFormat="1" ht="12">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="43"/>
+      <c r="E19" s="41"/>
     </row>
     <row r="20" spans="1:5" s="9" customFormat="1" ht="12">
       <c r="A20" s="10"/>
@@ -6434,7 +6469,7 @@
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
       <c r="D55" s="15"/>
-      <c r="E55" s="44"/>
+      <c r="E55" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6463,96 +6498,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -7223,6 +7258,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
@@ -7231,11 +7271,6 @@
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -7259,96 +7294,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -8095,12 +8130,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
@@ -8108,6 +8137,12 @@
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -8131,96 +8166,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -8872,6 +8907,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -8880,11 +8920,6 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -8908,96 +8943,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>423</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -9560,6 +9595,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -9568,15 +9608,10 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="92" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="93" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;A &amp;P/&amp;N</oddFooter>
   </headerFooter>
@@ -9596,96 +9631,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -10254,6 +10289,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -10262,15 +10302,10 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="92" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="93" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;A &amp;P/&amp;N</oddFooter>
   </headerFooter>
@@ -10290,96 +10325,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>222</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -10576,7 +10611,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="36" t="s">
         <v>457</v>
       </c>
       <c r="B30" s="3"/>
@@ -10600,7 +10635,7 @@
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
       <c r="F34" s="30"/>
-      <c r="G34" s="38" t="s">
+      <c r="G34" s="37" t="s">
         <v>461</v>
       </c>
       <c r="H34" s="22"/>
@@ -10625,7 +10660,7 @@
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="38" t="s">
+      <c r="G35" s="37" t="s">
         <v>460</v>
       </c>
       <c r="H35" s="22"/>
@@ -10645,6 +10680,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
@@ -10653,15 +10693,10 @@
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="92" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="93" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;A &amp;P/&amp;N</oddFooter>
   </headerFooter>
@@ -10679,96 +10714,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -11352,7 +11387,7 @@
       </c>
     </row>
     <row r="67" spans="1:21">
-      <c r="A67" s="37" t="s">
+      <c r="A67" s="36" t="s">
         <v>457</v>
       </c>
       <c r="B67" s="3"/>
@@ -11372,7 +11407,7 @@
       <c r="D71" s="29"/>
       <c r="E71" s="29"/>
       <c r="F71" s="30"/>
-      <c r="G71" s="38" t="s">
+      <c r="G71" s="37" t="s">
         <v>464</v>
       </c>
       <c r="H71" s="22"/>
@@ -11397,7 +11432,7 @@
       <c r="D72" s="18"/>
       <c r="E72" s="18"/>
       <c r="F72" s="19"/>
-      <c r="G72" s="39" t="s">
+      <c r="G72" s="38" t="s">
         <v>465</v>
       </c>
       <c r="H72" s="22"/>
@@ -11436,7 +11471,7 @@
       <c r="D78" s="29"/>
       <c r="E78" s="29"/>
       <c r="F78" s="30"/>
-      <c r="G78" s="38" t="s">
+      <c r="G78" s="37" t="s">
         <v>467</v>
       </c>
       <c r="H78" s="22"/>
@@ -11461,7 +11496,7 @@
       <c r="D79" s="18"/>
       <c r="E79" s="18"/>
       <c r="F79" s="19"/>
-      <c r="G79" s="39" t="s">
+      <c r="G79" s="38" t="s">
         <v>465</v>
       </c>
       <c r="H79" s="22"/>
@@ -11481,11 +11516,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="J2:Q2"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="U2:X2"/>
@@ -11494,6 +11524,11 @@
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="J2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -11516,96 +11551,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -12219,6 +12254,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
@@ -12226,12 +12267,6 @@
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -12254,96 +12289,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -12959,6 +12994,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -12967,11 +13007,6 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -12994,96 +13029,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -13756,6 +13791,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -13764,11 +13804,6 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -13791,96 +13826,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -14599,6 +14634,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -14607,11 +14647,6 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -14634,96 +14669,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -15933,6 +15968,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
@@ -15941,11 +15981,6 @@
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -15968,96 +16003,96 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="35" width="3.109375" customWidth="1"/>
+    <col min="1" max="35" width="3.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="53" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="50" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="55"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="50" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="50" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="55"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="54"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -16689,6 +16724,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
@@ -16697,11 +16737,6 @@
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -16714,21 +16749,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101007605912F2D65D948A2D62A06926ABED8" ma:contentTypeVersion="0" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="dfd4cfe015fbbeff87d046a03120f855">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0cd854ec148d7fa3f28b696a2ee3dff9">
     <xsd:element name="properties">
@@ -16842,10 +16862,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C16F3BC9-CFD2-403C-9D57-3DD46D5A4BDD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62DDAB71-9EDF-4F5A-B4D7-E12B105B94F6}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -16860,16 +16902,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62DDAB71-9EDF-4F5A-B4D7-E12B105B94F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C16F3BC9-CFD2-403C-9D57-3DD46D5A4BDD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
add : user edit activity
</commit_message>
<xml_diff>
--- a/Android/03_基本設計書(Android).xlsx
+++ b/Android/03_基本設計書(Android).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2220177\AndroidStudioProjects\Whisper\Android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5669DB4-30F0-4655-A999-9E1F44595457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F0C081-0AB5-469F-AF58-CD4E2C35BC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4725,6 +4725,11 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4740,6 +4745,15 @@
     <xf numFmtId="56" fontId="7" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4749,22 +4763,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5942,7 +5942,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="11"/>
@@ -5958,30 +5958,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
       <c r="C1" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="E1" s="48"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" ht="26.4" customHeight="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="52" t="s">
         <v>472</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="53"/>
       <c r="C2" s="39" t="s">
         <v>474</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="54">
         <v>45008</v>
       </c>
-      <c r="E2" s="50"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="4" spans="1:5" ht="11.5" thickBot="1">
       <c r="A4" s="6" t="s">
@@ -6004,16 +6004,16 @@
       <c r="A5" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="48" t="s">
         <v>477</v>
       </c>
     </row>
@@ -6066,16 +6066,16 @@
       <c r="A9" s="10">
         <v>5</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" ht="12">
       <c r="A10" s="10">
@@ -6504,90 +6504,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -7258,11 +7258,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
@@ -7271,6 +7266,11 @@
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -7300,90 +7300,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -8130,6 +8130,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
@@ -8137,12 +8143,6 @@
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -8172,90 +8172,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -8907,11 +8907,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -8920,6 +8915,11 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -8949,90 +8949,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>423</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -9595,11 +9595,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -9608,6 +9603,11 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -9637,90 +9637,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -10289,11 +10289,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -10302,6 +10297,11 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -10331,90 +10331,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -10680,11 +10680,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
@@ -10693,6 +10688,11 @@
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -10720,90 +10720,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -11516,6 +11516,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="J2:Q2"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="U2:X2"/>
@@ -11524,11 +11529,6 @@
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
     <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="J2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -11557,90 +11557,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -12254,12 +12254,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
@@ -12267,6 +12261,12 @@
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -12295,90 +12295,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -12994,11 +12994,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -13007,6 +13002,11 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -13035,90 +13035,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -13791,11 +13791,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -13804,6 +13799,11 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -13832,90 +13832,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -14634,11 +14634,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:X1"/>
@@ -14647,6 +14642,11 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -14675,90 +14675,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -15968,11 +15968,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
@@ -15981,6 +15976,11 @@
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -16009,90 +16009,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="57" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="52" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="54"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="55" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="52" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="57" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="57" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="1"/>
@@ -16724,11 +16724,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:X1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:Q2"/>
@@ -16737,6 +16732,11 @@
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -16749,6 +16749,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101007605912F2D65D948A2D62A06926ABED8" ma:contentTypeVersion="0" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="dfd4cfe015fbbeff87d046a03120f855">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0cd854ec148d7fa3f28b696a2ee3dff9">
     <xsd:element name="properties">
@@ -16862,32 +16877,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62DDAB71-9EDF-4F5A-B4D7-E12B105B94F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C16F3BC9-CFD2-403C-9D57-3DD46D5A4BDD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -16902,9 +16895,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C16F3BC9-CFD2-403C-9D57-3DD46D5A4BDD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62DDAB71-9EDF-4F5A-B4D7-E12B105B94F6}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>